<commit_message>
add unit test for create folder feat
</commit_message>
<xml_diff>
--- a/tests/dummy_company_data.xlsx
+++ b/tests/dummy_company_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bf09d77fea5249cc/NP/Year 3.2/DevOps/testing/Flask4Python/tests/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bf09d77fea5249cc/NP/Year 3.2/DevOps/testing/Flask4Python/uploaded_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="8_{052B822A-BB87-4F82-8153-8B67F3E75A6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A8770EA0-17AF-429D-AA93-850D40F90FBA}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="8_{052B822A-BB87-4F82-8153-8B67F3E75A6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FF344365-63F0-48A0-8CBF-F01172A26569}"/>
   <bookViews>
-    <workbookView xWindow="15780" yWindow="8265" windowWidth="11400" windowHeight="6990" xr2:uid="{A13D96F5-40AA-4A95-81D3-1E5055213CF6}"/>
+    <workbookView xWindow="7095" yWindow="8130" windowWidth="17415" windowHeight="9675" xr2:uid="{A13D96F5-40AA-4A95-81D3-1E5055213CF6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -53,28 +53,28 @@
     <t>Software Engineer</t>
   </si>
   <si>
+    <t>A inc.</t>
+  </si>
+  <si>
     <t>John Smith</t>
   </si>
   <si>
+    <t>john@abc.com</t>
+  </si>
+  <si>
+    <t>B Inc.</t>
+  </si>
+  <si>
     <t>Sum Ting Wong</t>
   </si>
   <si>
+    <t>sum@abc.com</t>
+  </si>
+  <si>
+    <t>C Inc.</t>
+  </si>
+  <si>
     <t>Michael Jack's Son</t>
-  </si>
-  <si>
-    <t>A inc.</t>
-  </si>
-  <si>
-    <t>B Inc.</t>
-  </si>
-  <si>
-    <t>C Inc.</t>
-  </si>
-  <si>
-    <t>john@abc.com</t>
-  </si>
-  <si>
-    <t>sum@abc.com</t>
   </si>
   <si>
     <t>michael@abc.com</t>
@@ -447,7 +447,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -473,41 +473,41 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -515,11 +515,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{540FF009-F370-493A-A8BF-0D50154AB3A6}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{4150413E-832A-44D5-AB49-5B3A29D2FB51}"/>
-    <hyperlink ref="D4" r:id="rId3" xr:uid="{40B2205E-545D-4FD9-95EA-50A2E24D6C1F}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{BD2E15DC-010B-4DDE-8982-BAF8DD49766F}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{FDE78B6C-1FE9-4DA8-9029-21198B9C98D8}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{2AEBC1DD-25EA-451F-8B3A-B0A11118BC12}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>